<commit_message>
Continued work on ticket importer
</commit_message>
<xml_diff>
--- a/templates/Tickets.xlsx
+++ b/templates/Tickets.xlsx
@@ -59,6 +59,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">The group to assign the ticket to. A ticket requires at least a group or a user. If you provide one, you do not need to provide the other.</t>
         </r>
@@ -112,7 +113,35 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
+          <t xml:space="preserve">Insert a list of category IDs here, separated by comma.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
           <t xml:space="preserve">An initial comment to open the ticket with. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">You can continue to add additional comments as additional columns, including and after this one. This allows you to insert as many comments as you want on a ticket.
+</t>
         </r>
       </text>
     </comment>
@@ -121,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -141,7 +170,13 @@
     <t xml:space="preserve">Priority</t>
   </si>
   <si>
+    <t xml:space="preserve">Category IDs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Initial Comment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Additional Comments</t>
   </si>
 </sst>
 </file>
@@ -151,7 +186,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -175,6 +210,7 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="0"/>
     </font>
@@ -184,11 +220,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -341,9 +372,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>19080</xdr:colOff>
+      <xdr:colOff>18720</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>104760</xdr:rowOff>
+      <xdr:rowOff>104400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -353,7 +384,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="77040" y="720"/>
-          <a:ext cx="6971400" cy="5956200"/>
+          <a:ext cx="5342040" cy="5955840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -426,46 +457,6 @@
               </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>Ticket comments can be imported in a separate importer.</a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:uFill>
-              <a:solidFill>
-                <a:srgbClr val="ffffff"/>
-              </a:solidFill>
-            </a:uFill>
-            <a:latin typeface="Times New Roman"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
             <a:t>Grey columns are required, blue columns are optional.</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
@@ -495,10 +486,13 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="1" sqref="H7:H8 L15"/>
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -516,24 +510,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H7:H8"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.8673469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7142857142857"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,8 +550,14 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add an option to import tickets as closed
</commit_message>
<xml_diff>
--- a/templates/Tickets.xlsx
+++ b/templates/Tickets.xlsx
@@ -145,12 +145,25 @@
         </r>
       </text>
     </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Set this to 0 to import the ticket as closed, 1 to import as open.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -177,6 +190,9 @@
   </si>
   <si>
     <t xml:space="preserve">Additional Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open</t>
   </si>
 </sst>
 </file>
@@ -372,9 +388,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>18720</xdr:colOff>
+      <xdr:colOff>18360</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>104400</xdr:rowOff>
+      <xdr:rowOff>104040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -384,7 +400,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="77040" y="720"/>
-          <a:ext cx="5342040" cy="5955840"/>
+          <a:ext cx="5256000" cy="5955480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -491,7 +507,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -510,25 +526,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0663265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7142857142857"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4336734693878"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -558,6 +574,9 @@
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restructure the ticket importer to make more sense.
</commit_message>
<xml_diff>
--- a/templates/Tickets.xlsx
+++ b/templates/Tickets.xlsx
@@ -140,21 +140,21 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
+          <t xml:space="preserve">1 for open, 0 for closed. Defaults to open if left blank.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
           <t xml:space="preserve">You can continue to add additional comments as additional columns, including and after this one. This allows you to insert as many comments as you want on a ticket.
 </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Set this to 0 to import the ticket as closed, 1 to import as open.</t>
         </r>
       </text>
     </comment>
@@ -189,10 +189,10 @@
     <t xml:space="preserve">Initial Comment</t>
   </si>
   <si>
+    <t xml:space="preserve">Open</t>
+  </si>
+  <si>
     <t xml:space="preserve">Additional Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open</t>
   </si>
 </sst>
 </file>
@@ -388,9 +388,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>18360</xdr:colOff>
+      <xdr:colOff>18000</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -400,7 +400,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="77040" y="720"/>
-          <a:ext cx="5256000" cy="5955480"/>
+          <a:ext cx="5255640" cy="5955120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -501,18 +501,18 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.37"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -528,23 +528,23 @@
   </sheetPr>
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="20.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="24.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -575,14 +575,14 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Add an option to the ticket import to import due dates
</commit_message>
<xml_diff>
--- a/templates/Tickets.xlsx
+++ b/templates/Tickets.xlsx
@@ -153,6 +153,19 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
+          <t xml:space="preserve">If this ticket has a due date, enter it here in YYYY-MM-DD format.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
           <t xml:space="preserve">You can continue to add additional comments as additional columns, including and after this one. This allows you to insert as many comments as you want on a ticket.
 </t>
         </r>
@@ -163,7 +176,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -388,9 +401,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>18000</xdr:colOff>
+      <xdr:colOff>17640</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>103320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -400,7 +413,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="77040" y="720"/>
-          <a:ext cx="5255640" cy="5955120"/>
+          <a:ext cx="5255280" cy="5954760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -526,25 +539,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="20.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="24.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -576,8 +591,12 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="L1" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Remove duplicate due date definition
</commit_message>
<xml_diff>
--- a/templates/Tickets.xlsx
+++ b/templates/Tickets.xlsx
@@ -153,19 +153,6 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">If this ticket has a due date, enter it here in YYYY-MM-DD format.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
           <t xml:space="preserve">You can continue to add additional comments as additional columns, including and after this one. This allows you to insert as many comments as you want on a ticket.
 </t>
         </r>
@@ -176,7 +163,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Subject</t>
   </si>
@@ -401,9 +388,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>17640</xdr:colOff>
+      <xdr:colOff>17280</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>103320</xdr:rowOff>
+      <xdr:rowOff>102960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -413,7 +400,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="77040" y="720"/>
-          <a:ext cx="5255280" cy="5954760"/>
+          <a:ext cx="5254920" cy="5954400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -539,10 +526,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:AMJ1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -554,12 +541,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="20.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="24.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="16.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="24.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -591,12 +576,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>